<commit_message>
created test cases for device module,executed auto connect and get_support(entervpn)
</commit_message>
<xml_diff>
--- a/exec/enter_vpn_windows/report_summary.xlsx
+++ b/exec/enter_vpn_windows/report_summary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\enter_vpn_windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A34105-D4A5-43BD-A760-A0F248CD7A81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE03EB77-49A2-4392-BC1A-16FAEB6B83DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="server_list" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="get_support" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="server_list" sheetId="1" r:id="rId3"/>
+    <sheet name="my_account" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>1. Log-in</t>
   </si>
@@ -111,6 +112,12 @@
   </si>
   <si>
     <t>TC_SYM_MA_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary(12-02-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_GSF_0021</t>
   </si>
 </sst>
 </file>
@@ -538,6 +545,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1826DD52-0D0B-4546-80C8-B2558CF2D6CA}">
+  <dimension ref="C2:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA10FA30-C202-4E11-BDE6-8D5A5E86909E}">
   <dimension ref="B1:B19"/>
   <sheetViews>
@@ -650,7 +725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C8"/>
   <sheetViews>
@@ -720,12 +795,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2717222-4177-4ABA-B79D-1AEA00CED8DA}">
   <dimension ref="C2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>